<commit_message>
Project stage 2 v0
</commit_message>
<xml_diff>
--- a/Tasks List.xlsx
+++ b/Tasks List.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Member</t>
   </si>
@@ -25,22 +25,46 @@
     <t>Complete Date</t>
   </si>
   <si>
+    <t>All</t>
+  </si>
+  <si>
     <t>Add more records to the database</t>
   </si>
   <si>
+    <t xml:space="preserve">Arpit </t>
+  </si>
+  <si>
     <t>Make login page</t>
   </si>
   <si>
     <t>Make registration page</t>
   </si>
   <si>
+    <t>Ishika</t>
+  </si>
+  <si>
     <t>Make forgot password page</t>
   </si>
   <si>
-    <t>Design registration page</t>
-  </si>
-  <si>
     <t>Design report on billing</t>
+  </si>
+  <si>
+    <t>Tri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make upcoming trips </t>
+  </si>
+  <si>
+    <t>Maeve</t>
+  </si>
+  <si>
+    <t>Delete reservations</t>
+  </si>
+  <si>
+    <t>Edit reservations</t>
+  </si>
+  <si>
+    <t>Test the pages</t>
   </si>
 </sst>
 </file>
@@ -304,7 +328,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="32.14"/>
+    <col customWidth="1" min="2" max="2" width="34.43"/>
     <col customWidth="1" min="3" max="3" width="14.14"/>
   </cols>
   <sheetData>
@@ -345,33 +369,75 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
+      <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="B5" s="3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
+      <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="B6" s="3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7">
+      <c r="A7" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="B7" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Project stage 2 v2
</commit_message>
<xml_diff>
--- a/Tasks List.xlsx
+++ b/Tasks List.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>Member</t>
   </si>
@@ -31,6 +31,9 @@
     <t>Add more records to the database</t>
   </si>
   <si>
+    <t>In progress</t>
+  </si>
+  <si>
     <t xml:space="preserve">Arpit </t>
   </si>
   <si>
@@ -49,42 +52,51 @@
     <t>Design report on billing</t>
   </si>
   <si>
+    <t>Maeve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make upcoming trips </t>
+  </si>
+  <si>
+    <t>Edit &amp; Delete reservations</t>
+  </si>
+  <si>
     <t>Tri</t>
   </si>
   <si>
-    <t xml:space="preserve">Make upcoming trips </t>
-  </si>
-  <si>
-    <t>Maeve</t>
-  </si>
-  <si>
-    <t>Delete reservations</t>
-  </si>
-  <si>
-    <t>Edit reservations</t>
+    <t>Account Page</t>
   </si>
   <si>
     <t>Test the pages</t>
+  </si>
+  <si>
+    <t>Search Page</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+  </numFmts>
   <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -101,7 +113,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -110,6 +122,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -326,10 +341,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="34.43"/>
-    <col customWidth="1" min="3" max="3" width="14.14"/>
+    <col customWidth="1" min="2" max="2" width="30.13"/>
+    <col customWidth="1" min="3" max="3" width="12.38"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -375,69 +390,134 @@
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D2" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="C3" s="4">
+        <v>44594.0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>44645.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="C4" s="4">
+        <v>44594.0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>44645.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="C5" s="4">
+        <v>44594.0</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C6" s="4">
+        <v>44638.0</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="C7" s="4">
+        <v>44638.0</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="C8" s="4">
+        <v>44638.0</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="C9" s="4">
+        <v>44639.0</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="C10" s="4">
+        <v>44594.0</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="4">
+        <v>44638.0</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>